<commit_message>
add 4 more 6-8night
</commit_message>
<xml_diff>
--- a/continental_2018-6-8晚.xlsx
+++ b/continental_2018-6-8晚.xlsx
@@ -11,13 +11,17 @@
     <sheet name="速平江衛" sheetId="2" r:id="rId2"/>
     <sheet name="沙里灣泥" sheetId="3" r:id="rId3"/>
     <sheet name="毛憐衛" sheetId="4" r:id="rId4"/>
+    <sheet name="坤城" sheetId="5" r:id="rId5"/>
+    <sheet name="嘔罕河衛" sheetId="6" r:id="rId6"/>
+    <sheet name="喜楽温河衛" sheetId="7" r:id="rId7"/>
+    <sheet name="哥吉河衛(哥吉阿衛)" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230">
   <si>
     <t>欽真河衛</t>
   </si>
@@ -35,6 +39,46 @@
   </si>
   <si>
     <r>
+      <t>哥吉河衛</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> /</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>哥吉阿衛</t>
+    </r>
+  </si>
+  <si>
+    <t>9(0)</t>
+  </si>
+  <si>
+    <t>喜楽温河衛</t>
+  </si>
+  <si>
+    <t>嘔罕河衛</t>
+  </si>
+  <si>
+    <t>坤城</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
       <t>英宗／卷一百三十七　正統十一年正月／</t>
     </r>
     <r>
@@ -50,6 +94,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
         <charset val="1"/>
       </rPr>
       <t>日</t>
@@ -72,6 +117,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <charset val="1"/>
+      </rPr>
       <t>憲宗／卷一百二十三　成化九年十二月／</t>
     </r>
     <r>
@@ -87,6 +138,7 @@
       <rPr>
         <sz val="10"/>
         <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
         <charset val="1"/>
       </rPr>
       <t>日</t>
@@ -545,6 +597,210 @@
   <si>
     <t>壬午毛憐衞都督同知李撒滿荅失里等來朝貢珠五百顆上諭行在禮部曰先王盛時四夷之獻惟服食器用珠于國用何益曩已諭緣邊總兵官凡諸夷來貢獻者不用珍玩今撒滿荅失里乃復貢珠本欲卻之第念遠人輸誠姑酬其直毋以為例</t>
   </si>
+  <si>
+    <t>宣宗／卷八　洪熙元年八月下／27日(P.216)</t>
+  </si>
+  <si>
+    <t>癸巳趙王高燧奏請躬祭献陵上以藩屏事重復書止之　行在禮部奏坤城等處使臣馬力丁等十五人進馬及方物復以馬來市上曰遠人宜厚待之凡賜鈔八千五百一十錠綵幣九十一表裡襍色絹二百三十匹綿布七十疋　賜哈密忠義王使臣賽因等二人鈔幣　太白晝見</t>
+  </si>
+  <si>
+    <t>宣宗／卷三十五　宣德三年正月／10日(P.877)</t>
+  </si>
+  <si>
+    <t>癸巳遣內官李信林春李貴郭泰等齎勑及金織文綺表裏往亦力把里別失把里亦昔闊哈烈馬綽兒八剌黑城把荅失罕撒馬兒罕賽藍城掃郎城達失干城失剌思亦思弗罕及坤城等處賜其王及頭目盖嘉其遣使朝貢也以信等道過沙州赤斤蒙古二衛併賜掌衛事都指揮僉事困即來指揮薛迭古等金織文綺綵幣有差</t>
+  </si>
+  <si>
+    <t>宣宗／卷六十三　宣德五年二月／7日(P.1477)</t>
+  </si>
+  <si>
+    <t>戊寅朝鮮國王李祹遣陪臣徐選貴州宣慰使安中遣弟喜安中遣弟喜:廣本禮本中作忠，誤。廣本禮本喜作加；抱本作嘉。按本卷第九頁後四行各本作嘉。乖西蠻夷長官司長官楊暹四川烏蒙軍民府土官祿昭祿昭:廣本昭誤招。本卷第九頁後五行各本作昭。雲南楚雄府女土官設劄坤城回回馬兒丁等貢馬及方物賀　萬壽聖節　廣西太平府土官知府張高歸德州土官知州黃高四川石柱宣撫司同知陳玘遣舍人陳伯州等貢馬　賜迤北和寧使臣脫火歹等六十二人鈔綵幣表裏有差</t>
+  </si>
+  <si>
+    <t>宣宗／卷六十三　宣德五年二月／22日(P.1488)</t>
+  </si>
+  <si>
+    <t>癸巳賜貴州宣慰使安中弟嘉乖西蠻夷長官司長官楊暹四川石柱宣撫司舍人陳伯舟烏蒙軍民府土官祿昭廣西太平府土官知府張高歸德州土官知州黃高雲南楚雄府女土官設劄坤城回回馬兒丁等鈔綵幣表裏及絹有差</t>
+  </si>
+  <si>
+    <t>宣宗／卷六十五　宣德五年四月／4日(P.1529)</t>
+  </si>
+  <si>
+    <t>甲戌坤城等處使臣者馬力丁等貢駝馬</t>
+  </si>
+  <si>
+    <t>宣宗／卷六十五　宣德五年四月／9日(P.1533)</t>
+  </si>
+  <si>
+    <t>己卯賜瓦剌坤城等處貢使脫火歹等宴</t>
+  </si>
+  <si>
+    <t>宣宗／卷六十五　宣德五年四月／18日(P.1540)</t>
+  </si>
+  <si>
+    <t>戊子賜坤城等處使臣者馬力丁等二十四人哈密忠順王所差奏事指揮捨黑馬黑麻等二人綵幣紵絲表裏絹有差</t>
+  </si>
+  <si>
+    <t>宣宗／卷六十七　宣德五年六月／11日(P.1578)</t>
+  </si>
+  <si>
+    <t>庚辰行在戶部奏坤城回回者馬兒丁等朝貢至京輸米一萬六千七百六十石于京倉中塩今者馬兒丁等欲還坤城言願以所納米獻官　上曰彼名為朝貢實務市易盖回回善營利也其米亦費本遠方之人可償其直于是戶部計直當以布八千疋絹四千疋償之從之</t>
+  </si>
+  <si>
+    <t>宣宗／卷八十三　宣德六年九月／6日(P.1913)</t>
+  </si>
+  <si>
+    <t>丁卯兀者前衞女直頭目巴領葛坤城使臣者馬里丁等來朝奏願居京自劾賜紵絲襲衣鈔布仍命有司給房屋器物如例</t>
+  </si>
+  <si>
+    <t>嘔罕河衞</t>
+  </si>
+  <si>
+    <t>宣宗／卷一百八　宣德九年正月至二月／正月／9日(P.2409)</t>
+  </si>
+  <si>
+    <t>丁亥肥河衛指揮使剌令哈遣指揮僉事牙當嘔罕河衛指揮使乃胯遣指揮僉事晏答等來朝貢馬</t>
+  </si>
+  <si>
+    <t>宣宗／卷一百八　宣德九年正月至二月／二月／5日(P.2419)</t>
+  </si>
+  <si>
+    <t>癸丑賜益實衛指揮僉事魯省奇失真奇及肥河衛指揮使剌令哈所遣指揮僉事牙當嘔罕河衛指揮僉事晏答等綵幣絹布及金織襲衣有差仍命牙當等齎勑及綵幣歸賜剌令哈</t>
+  </si>
+  <si>
+    <t>英宗／卷十四　正統元年二月／29日(P.273)</t>
+  </si>
+  <si>
+    <t>乙丑陞嘔罕河衛都指揮僉事乃胯為都指揮同知右城衛指揮使木答兀益實衛指揮木當哈為都指揮僉事也孫倫衛指揮同知卜不剌考郎兀衛指揮同知薛列河為指揮使朵林山衛指揮僉事扯養加忽魯愛衛指揮僉事苦出納禿都河衛指揮僉事也兒哥也兒哥:中本作也哥兒。老哈河衛指揮僉事八思㙮八思㙮:抱本㙮作㗳。為指揮同知渚冬河衛百戶演不花為副千戶可令河等衛頭目歹羊加等十一人俱授副千戶以乃胯等來朝援例奏請也</t>
+  </si>
+  <si>
+    <t>英宗／卷十七　正統元年五月／21日(P.337)</t>
+  </si>
+  <si>
+    <t>丙戌嘔罕河衛女直指揮古已柰雲南景東雲南景東:廣本抱本中本東下有府字，是也。把事姜崐尋甸軍民府把事男楊恕楚雄府把事王斌廣西忠州土官知州王志王志:廣本抱本中本王志作黃智。并太平府左州俱遣人來朝貢馬及方物賜宴并綵幣等物有差</t>
+  </si>
+  <si>
+    <t>英宗／卷二十四　正統元年十一月／16日(P.479)</t>
+  </si>
+  <si>
+    <t>丁未泰寧衛都督僉事拙赤海西嘔罕河衛野人女直路失等兀者衛野人都指揮剌㙮古脫倫衛野人忽里并加古賁葛林阿剌山奇吉河奇吉河:抱本吉作古。婆羅河亦罕河六衛女直兀的納等并雲南洱海衛女土官高氏湖廣搖把峒長司土官長司土官:廣本抱本長下有官字，是也。向墨等俱來朝貢馬及方物賜宴并賜綵幣等物有差</t>
+  </si>
+  <si>
+    <t>英宗／卷二十五　正統元年十二月／17日(P.500)</t>
+  </si>
+  <si>
+    <t>戊寅四川播州宣慰使楊昇遣長官楊勝宗等并哈剌孩等衛女直指揮吉列兒等嘔罕河衛女直指揮脫因托兀者前等衛女直指揮阿剌禿等各來朝貢鷹馬及方物賜宴并賜綵幣等物有差　命山東濟南府濱州知州梁昭復任昭在濱州鋤擊姦豪撫恤窮民以母喪去任州民聞昭服闋相率赴京奏保故復之</t>
+  </si>
+  <si>
+    <t>英宗／卷二十七　正統二年二月／4日(P.534)</t>
+  </si>
+  <si>
+    <t>甲子命嘔罕河衛指揮吉當加齎敕及金織襲衣綵幣歸賜其頭目指揮乃胯</t>
+  </si>
+  <si>
+    <t>英宗／卷五十　正統四年正月／8日(P.961)</t>
+  </si>
+  <si>
+    <t>丁亥朝鮮國王李祹遣陪臣尹延命等奉表貢方物謝恩福餘等衞指揮帖木兒薛列河衞指揮革同哥朵顏衞指揮孛羅失里木衞女直舍人哈丁加泰寧衞指揮咬脫歡嘔罕河衞女直舍人丹八廣西太平府龍英州官簇官簇:抱本簇作族。趙安等俱來朝貢馬駝及方物賜宴并綵幣等物有差</t>
+  </si>
+  <si>
+    <t>英宗／卷五十九　正統四年九月／4日(P.1129)</t>
+  </si>
+  <si>
+    <t>己酉琉球國遣使臣李敬占城國遣使臣逋沙怕濟閣并牙魯衛女直指揮阿省哥愛和衛女直指揮已失兀者衛野人女直舍人阿的納督罕河衛女直指揮滿古亦文山衛女直指揮斡欒哥納剌吉河衛頭目賽因加兀賴忽衛頭目色路合兀魯罕河衛兀魯罕河衞:抱本兀誤元。會典卷一百二十五作兀。舍人土申加阿真河衛舍人省失嘔罕河衛指揮阿都赤等俱來朝貢馬及方物賜宴并賜綵幣等物有差</t>
+  </si>
+  <si>
+    <t>英宗／卷七十六　正統六年二月／12日(P.1489)</t>
+  </si>
+  <si>
+    <t>己卯遼東建州左衛女直指揮易使加易使加:廣本抱本使作失。等嘔罕河衛女直指揮帖木兒哈考郎兀衛女直指揮古郎加等愛河衛野人女直阿塔出雲南順寧府土官知府猛盖遣把事馬塝四川建昌衛昌州長官司土官長官盧聚遣把事阿苴俱來朝貢馬及方物賜宴并賜綵幣等物有差</t>
+  </si>
+  <si>
+    <t>英宗／卷七十六　正統六年二月／20日(P.1501)</t>
+  </si>
+  <si>
+    <t>丁亥陞嘔罕河衛都指揮同知乃胯為都督僉事以乃胯遣本衛指揮帖木兒等八人進馬請陞也</t>
+  </si>
+  <si>
+    <t>孝宗／卷七十二　弘治六年二月／10日(P.1347)</t>
+  </si>
+  <si>
+    <t>乙巳弗提衞都督答只祿亦把哈及嘔罕河衞都督尚古各來貢賜宴并衣服綵叚等物有差三人復各陳父祖以來多效勞邊塞乞加賞賚命賜答只祿蟒衣亦把哈及尚古金帶冠帽各一事</t>
+  </si>
+  <si>
+    <t>武宗／卷一百四十七　正德十二年三月／14日(P.2867)</t>
+  </si>
+  <si>
+    <t>己丑海西嘔罕河衛夷人褚飬哈等入貢道永平擾害驛逓遼東伴送舍人傅鐸奏之禮部議覆詔大通事譯審明白嚴加撫諭禮部仍量差通事送歸既而海西兀者等衛夷幹黑能等歸伴送舍人亦請遣通事護送許之遂著為令</t>
+  </si>
+  <si>
+    <t>世宗／卷一百六十　嘉靖十三年閏二月／5日(P.3573)</t>
+  </si>
+  <si>
+    <t>壬寅海西嘔罕河衛女直左都督左都督:閣本無左字。褚養哈等來朝貢馬給賞如例</t>
+  </si>
+  <si>
+    <t>附錄／明武宗寶訓／卷二／優遠人／正德十二年三月14日(P.187)</t>
+  </si>
+  <si>
+    <t>己丑海西嘔罕河衞夷人褚飬哈等人貢道永平擾害驛逓遼東伴送舍人傅鐸奏之禮部議覆詔大通事譯審明白嚴加撫諭禮部仍量差通事送歸既而海西兀者等衛夷斡黑能等歸伴送舍人亦請遣通事護送遂著為令</t>
+  </si>
+  <si>
+    <t>哥吉河衞</t>
+  </si>
+  <si>
+    <t>宣宗／卷二十五　宣德二年二月／17日(P.658)</t>
+  </si>
+  <si>
+    <t>乙亥賜廣西田州府故土官舍人岑紹陜西洮州等衞土官百戶剌麻失寧卜蕭失寧卜蕭:廣本蕭作寧。及哥吉河衞舍人把失罕亦力把里回回打剌罕馬黑麻哈非思等鈔綵幣表裏紵絲襲衣綵幣表裏紵絲襲衣:廣本無紵絲二字，綵幣作紗羅。有差</t>
+  </si>
+  <si>
+    <t>宣宗／卷一百六　宣德八年九月至十月／九月／15日(P.2361)</t>
+  </si>
+  <si>
+    <t>甲午遣哥吉河衛差來指揮吉速你等等齎勑命其衛故指揮同知可成孫未希納襲職仍賜金織文綺襲衣</t>
+  </si>
+  <si>
+    <t>宣宗／卷一百十二　宣德九年八月至九月／八月／1日(P.2511)</t>
+  </si>
+  <si>
+    <t>乙巳朔哥吉河衛指揮同知末稀納剌蘭吉衛指揮同知我可哥福餘衛副千戶阿林台等來朝貢馬及方物</t>
+  </si>
+  <si>
+    <t>宣宗／卷一百十二　宣德九年八月至九月／八月／12日(P.2515)</t>
+  </si>
+  <si>
+    <t>丙辰賜哥吉河衛指揮同知末稀納剌蘭吉衛指揮同知我可哥福餘衛千戶福餘衞千戶:廣本抱本衞下有副字。阿林台等鈔幣絹布及紵絲襲衣有差</t>
+  </si>
+  <si>
+    <t>英宗／卷七十五　正統六年正月／22日(P.1470)</t>
+  </si>
+  <si>
+    <t>庚申命哥吉河衞指揮同知可成哥孫末希納襲職泰寧衞都督脫火赤子討勤襲為都指揮使授都督拙赤弟失南帖木兒為正千戶俱賜勑諭</t>
+  </si>
+  <si>
+    <t>英宗／卷七十五　正統六年正月／24日(P.1471)</t>
+  </si>
+  <si>
+    <t>壬戌哥吉河衞野人女直木帶木帶:抱本木作末。納朶倫衞女直滿哥自在州指揮兀丁哥陜西岷州衞番僧綱司廣福寺剌麻鎖南屋即等俱來朝貢馬賜綵叚表裏有差</t>
+  </si>
+  <si>
+    <t>英宗／卷一百二十三　正統九年十一月／14日(P.2463)</t>
+  </si>
+  <si>
+    <t>己丑滿剌加國遣使臣宋那的剌耶等福餘等衛指揮馬撒罕等亦里察河衛哥吉河衛哥吉河衞:廣本無此四字。兀者托溫千戶所野人亦里荅等俱來朝貢馬及方物賜宴及綵幣表裏鈔絹等物有差</t>
+  </si>
+  <si>
+    <t>英宗／卷一百八十六　廢帝郕戾王附錄第四　正統十四年十二月／27日(P.3763)</t>
+  </si>
+  <si>
+    <t>癸酉陞哥吉河衞都指揮僉事劄魯哈劄魯哈:廣本劄作劉。為都指揮同知童寬山衞指揮使住羊哈為都指揮僉事時邊塵未靖而二人躬來朝貢故特陞之</t>
+  </si>
+  <si>
+    <t>英宗／卷二百六十二　廢帝郕戾王附錄第八十　景泰七年正月／26日(P.5602)</t>
+  </si>
+  <si>
+    <t>丙申赤斤蒙古衛都督阿速指揮可兒加等來朝貢馬駝及方物賜宴及綵幣表裡襲衣鈔絹鈔絹:廣本鈔作紗。等物有差　陞刑部陜西司主事倪通為陜西按察司僉事江西司主事劉羽翔河南道監察御史陳敬俱為江西按察司僉事湖廣道監察御史張昊張昊:廣本昊作炅。為廣東按察司僉事　命故毛憐衛指揮使納刺禿子兀里哈指揮同知速都子塞籠格莽哈子謟護木答忽子鎖古奴答魯哈答魯哈:廣本答魯作合普。子卜郎把連子阿魯指揮僉事孫昌答子撦亦客荅哈答哈:廣本抱本作哈答。子塞列失保赤子帖黑車阿哈子兀察黃脫因子那那哈建州衛指揮使賽因不花賽因不花:廣本不作百。子撒哈答指揮同知冬鎖魯阿子煖塔塔失子撒哈刺忽失哈子你魯兒因你魯兒因:廣本抱本魯下有禿字。子塔養重山子双古奴指揮僉事丹保奴子把荅哈安赤哈安赤:廣本赤作察。子捏失格小廝子也迭乞也迭乞:廣本無乞字。失里木衛指揮僉事賽示塔賽示塔:廣本無示字。子板里塔咬納子亦失哈亦失哈:廣本無失字。抱本失下有失字。哥吉河衛指揮僉事准里亭哥准里亭哥:廣本里亭作呈停。子阿納哈八令哈子速失遼東自在州住坐指揮同知神干保子宮保神干保子宮保:廣本抱本宮作官。指揮僉事七十子五十俱襲職</t>
+  </si>
 </sst>
 </file>
 
@@ -556,7 +812,7 @@
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="31">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -567,6 +823,7 @@
     <font>
       <sz val="10.5"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <charset val="134"/>
     </font>
     <font>
@@ -589,10 +846,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
+      <name val="Calibri"/>
       <charset val="1"/>
     </font>
     <font>
@@ -602,23 +861,35 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -633,7 +904,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -646,9 +917,86 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -663,83 +1011,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -751,6 +1022,12 @@
       <name val="Arial"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -758,30 +1035,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -803,13 +1056,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -821,19 +1074,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -845,19 +1092,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -869,37 +1116,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -917,7 +1140,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,13 +1152,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -964,6 +1241,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -975,6 +1267,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1009,21 +1312,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1041,168 +1329,157 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="29" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1210,6 +1487,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
@@ -1222,6 +1503,15 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1538,13 +1828,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelCol="2"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
@@ -1579,7 +1869,7 @@
       </c>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C5">
@@ -1590,6 +1880,43 @@
       <c r="C6">
         <f>SUM(C1:C5)</f>
         <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="3:3">
+      <c r="C12">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1610,31 +1937,31 @@
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelRow="1" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>7</v>
+      <c r="B1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>7</v>
+      <c r="B2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1659,10 +1986,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1677,7 +2004,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A1" sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelCol="3"/>
@@ -1687,133 +2014,133 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3"/>
+        <v>20</v>
+      </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3"/>
+        <v>22</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>26</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>30</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="3"/>
+        <v>32</v>
+      </c>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>7</v>
+        <v>38</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1821,205 +2148,205 @@
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D14" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
-      </c>
-      <c r="D15" s="3"/>
+        <v>46</v>
+      </c>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="D16" s="5"/>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="D17" s="5"/>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>52</v>
+      </c>
+      <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>54</v>
+      </c>
+      <c r="D19" s="5"/>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="D20" s="5"/>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="D21" s="5"/>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="C22" t="s">
-        <v>55</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>60</v>
+      </c>
+      <c r="D22" s="5"/>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="C23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" s="3"/>
+        <v>62</v>
+      </c>
+      <c r="D23" s="5"/>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>59</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>64</v>
+      </c>
+      <c r="D24" s="5"/>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="C25" t="s">
-        <v>61</v>
-      </c>
-      <c r="D25" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="D25" s="5"/>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="C26" t="s">
-        <v>63</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>68</v>
+      </c>
+      <c r="D26" s="5"/>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
-      </c>
-      <c r="D27" s="3"/>
+        <v>70</v>
+      </c>
+      <c r="D27" s="5"/>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C28" t="s">
-        <v>67</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>7</v>
+        <v>72</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2027,61 +2354,61 @@
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="C29" t="s">
-        <v>69</v>
-      </c>
-      <c r="D29" s="3"/>
+        <v>74</v>
+      </c>
+      <c r="D29" s="5"/>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>71</v>
-      </c>
-      <c r="D30" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="D30" s="5"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C31" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="D31" s="5"/>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D32" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="D32" s="5"/>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C33" t="s">
-        <v>77</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>7</v>
+        <v>82</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2089,25 +2416,25 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="D34" s="5"/>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="C35" t="s">
-        <v>81</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2115,253 +2442,253 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" s="3"/>
+        <v>89</v>
+      </c>
+      <c r="D36" s="5"/>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" s="3"/>
+        <v>91</v>
+      </c>
+      <c r="D37" s="5"/>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="D38" s="5"/>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C39" t="s">
-        <v>90</v>
-      </c>
-      <c r="D39" s="3"/>
+        <v>95</v>
+      </c>
+      <c r="D39" s="5"/>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="C40" t="s">
-        <v>92</v>
-      </c>
-      <c r="D40" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="D40" s="5"/>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
-      </c>
-      <c r="D41" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="D41" s="5"/>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="C42" t="s">
-        <v>96</v>
-      </c>
-      <c r="D42" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="D42" s="5"/>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C43" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="D43" s="5"/>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C44" t="s">
-        <v>100</v>
-      </c>
-      <c r="D44" s="3"/>
+        <v>105</v>
+      </c>
+      <c r="D44" s="5"/>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C45" t="s">
-        <v>102</v>
-      </c>
-      <c r="D45" s="3"/>
+        <v>107</v>
+      </c>
+      <c r="D45" s="5"/>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="C46" t="s">
-        <v>104</v>
-      </c>
-      <c r="D46" s="3"/>
+        <v>109</v>
+      </c>
+      <c r="D46" s="5"/>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C47" t="s">
-        <v>106</v>
-      </c>
-      <c r="D47" s="3"/>
+        <v>111</v>
+      </c>
+      <c r="D47" s="5"/>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C48" t="s">
-        <v>108</v>
-      </c>
-      <c r="D48" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="D48" s="5"/>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="C49" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" s="3"/>
+        <v>115</v>
+      </c>
+      <c r="D49" s="5"/>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C50" t="s">
-        <v>112</v>
-      </c>
-      <c r="D50" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="D50" s="5"/>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
-        <v>114</v>
-      </c>
-      <c r="D51" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="D51" s="5"/>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
-        <v>116</v>
-      </c>
-      <c r="D52" s="3"/>
+        <v>121</v>
+      </c>
+      <c r="D52" s="5"/>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C53" t="s">
-        <v>118</v>
-      </c>
-      <c r="D53" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="D53" s="5"/>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C54" t="s">
-        <v>120</v>
-      </c>
-      <c r="D54" s="3"/>
+        <v>125</v>
+      </c>
+      <c r="D54" s="5"/>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C55" t="s">
-        <v>122</v>
-      </c>
-      <c r="D55" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="D55" s="5"/>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C56" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>7</v>
+        <v>129</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:4">
@@ -2369,192 +2696,661 @@
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C57" t="s">
-        <v>126</v>
-      </c>
-      <c r="D57" s="3"/>
+        <v>131</v>
+      </c>
+      <c r="D57" s="5"/>
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C58" t="s">
-        <v>128</v>
-      </c>
-      <c r="D58" s="3"/>
+        <v>133</v>
+      </c>
+      <c r="D58" s="5"/>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="C59" t="s">
-        <v>130</v>
-      </c>
-      <c r="D59" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="D59" s="5"/>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C60" t="s">
-        <v>132</v>
-      </c>
-      <c r="D60" s="3"/>
+        <v>137</v>
+      </c>
+      <c r="D60" s="5"/>
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C61" t="s">
-        <v>134</v>
-      </c>
-      <c r="D61" s="3"/>
+        <v>139</v>
+      </c>
+      <c r="D61" s="5"/>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C62" t="s">
-        <v>136</v>
-      </c>
-      <c r="D62" s="3"/>
+        <v>141</v>
+      </c>
+      <c r="D62" s="5"/>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C63" t="s">
-        <v>138</v>
-      </c>
-      <c r="D63" s="3"/>
+        <v>143</v>
+      </c>
+      <c r="D63" s="5"/>
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C64" t="s">
-        <v>140</v>
-      </c>
-      <c r="D64" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="D64" s="5"/>
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C65" t="s">
-        <v>142</v>
-      </c>
-      <c r="D65" s="3"/>
+        <v>147</v>
+      </c>
+      <c r="D65" s="5"/>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C66" t="s">
-        <v>144</v>
-      </c>
-      <c r="D66" s="3"/>
+        <v>149</v>
+      </c>
+      <c r="D66" s="5"/>
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C67" t="s">
-        <v>146</v>
-      </c>
-      <c r="D67" s="3"/>
+        <v>151</v>
+      </c>
+      <c r="D67" s="5"/>
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C68" t="s">
-        <v>148</v>
-      </c>
-      <c r="D68" s="3"/>
+        <v>153</v>
+      </c>
+      <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C69" t="s">
-        <v>150</v>
-      </c>
-      <c r="D69" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C70" t="s">
-        <v>152</v>
-      </c>
-      <c r="D70" s="3"/>
+        <v>157</v>
+      </c>
+      <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C71" t="s">
-        <v>154</v>
-      </c>
-      <c r="D71" s="3"/>
+        <v>159</v>
+      </c>
+      <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C72" t="s">
-        <v>156</v>
-      </c>
-      <c r="D72" s="3"/>
+        <v>161</v>
+      </c>
+      <c r="D72" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D10" s="4"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="D13" s="4"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D14" s="4"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D15" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.2" outlineLevelCol="3"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>